<commit_message>
fix - Pagination key
</commit_message>
<xml_diff>
--- a/output/resources/resources_changeLog.xlsx
+++ b/output/resources/resources_changeLog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>ENDPOINT</t>
   </si>
@@ -86,6 +86,15 @@
     <t>resources/</t>
   </si>
   <si>
+    <t>pagination-key</t>
+  </si>
+  <si>
+    <t>'pagination-key' adicionado;</t>
+  </si>
+  <si>
+    <t>get/parameters</t>
+  </si>
+  <si>
     <t>423</t>
   </si>
   <si>
@@ -242,13 +251,19 @@
     <t>'application/json; charset=utf-8' adicionado;</t>
   </si>
   <si>
-    <t>servers</t>
+    <t>servers/0</t>
   </si>
   <si>
     <t>url</t>
   </si>
   <si>
     <t>'url' alterado de 'https://api.banco.com.br/open-banking/resources/v1' para 'https://api.banco.com.br/open-banking/resources/v2';</t>
+  </si>
+  <si>
+    <t>servers/1</t>
+  </si>
+  <si>
+    <t>'url' alterado de 'https://apih.banco.com.br/open-banking/resources/v1' para 'https://apih.banco.com.br/open-banking/resources/v2';</t>
   </si>
 </sst>
 </file>
@@ -288,7 +303,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -355,7 +370,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -369,13 +384,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -397,13 +412,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -414,10 +429,10 @@
         <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -425,7 +440,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>26</v>
@@ -442,10 +457,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -453,13 +468,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -467,13 +482,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -481,13 +496,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -495,13 +510,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -509,13 +524,13 @@
         <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -523,13 +538,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -537,13 +552,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -551,13 +566,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -565,13 +580,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -579,13 +594,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -593,13 +608,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -607,13 +622,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -621,13 +636,13 @@
         <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -635,13 +650,13 @@
         <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -649,13 +664,13 @@
         <v>10</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -663,13 +678,13 @@
         <v>10</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -677,13 +692,13 @@
         <v>10</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -691,13 +706,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -705,13 +720,13 @@
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -719,13 +734,13 @@
         <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -733,13 +748,13 @@
         <v>10</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -747,13 +762,13 @@
         <v>10</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -761,13 +776,13 @@
         <v>10</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -775,13 +790,13 @@
         <v>10</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -789,13 +804,13 @@
         <v>10</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -803,13 +818,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -817,10 +832,10 @@
         <v>10</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>57</v>
@@ -831,13 +846,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -845,7 +860,7 @@
         <v>10</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>61</v>
@@ -856,16 +871,44 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>64</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>